<commit_message>
fixing back transformations and reformating plots for journal requirements
</commit_message>
<xml_diff>
--- a/plots/Fig2_DensityPlots/equationsToPercChangePerYr.xlsx
+++ b/plots/Fig2_DensityPlots/equationsToPercChangePerYr.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\elwel\OneDrive\Desktop\aquatic_data\git\EuroAquaticMacroInverts\plots\Fig2_DensityPlots\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99F1382B-9516-411E-94CD-B12F95A70C44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60A385ED-B436-4B14-A7C1-996103916EC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12948" yWindow="1608" windowWidth="9456" windowHeight="11028" xr2:uid="{070CE87A-CE06-49D1-A7CB-3F8E4BBDE3C6}"/>
+    <workbookView xWindow="3984" yWindow="1380" windowWidth="13380" windowHeight="11028" xr2:uid="{070CE87A-CE06-49D1-A7CB-3F8E4BBDE3C6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="34">
   <si>
     <t>MetaWeighted</t>
   </si>
@@ -127,6 +127,15 @@
   </si>
   <si>
     <t>logit (beta models)</t>
+  </si>
+  <si>
+    <t>Mean(Response^2)</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>back transformation calculated in script to create Fig. 2</t>
   </si>
 </sst>
 </file>
@@ -479,10 +488,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74D24C37-4EDC-4D52-AFA2-C59378FD0759}">
-  <dimension ref="A1:F21"/>
+  <dimension ref="A1:H21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="86" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -491,7 +500,7 @@
     <col min="2" max="2" width="18.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>21</v>
       </c>
@@ -505,13 +514,19 @@
         <v>29</v>
       </c>
       <c r="E1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F1" t="s">
         <v>24</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="H1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -524,15 +539,15 @@
       <c r="D2">
         <v>27.287123139999999</v>
       </c>
-      <c r="E2">
+      <c r="F2">
         <f>(C2/D2)*100</f>
         <v>0.7344252194407036</v>
       </c>
-      <c r="F2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -545,15 +560,15 @@
       <c r="D3">
         <v>19.245025900000002</v>
       </c>
-      <c r="E3">
-        <f t="shared" ref="E3:E4" si="0">(C3/D3)*100</f>
+      <c r="F3">
+        <f t="shared" ref="F3:F4" si="0">(C3/D3)*100</f>
         <v>0.22446032145895939</v>
       </c>
-      <c r="F3" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -566,15 +581,15 @@
       <c r="D4">
         <v>1.9782322990000001</v>
       </c>
-      <c r="E4">
+      <c r="F4">
         <f t="shared" si="0"/>
         <v>0.24848583265397384</v>
       </c>
-      <c r="F4" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>0</v>
       </c>
@@ -584,15 +599,15 @@
       <c r="C5">
         <v>-2.345967E-3</v>
       </c>
-      <c r="E5">
+      <c r="F5">
         <f>(10^C5-1)*100</f>
         <v>-0.5387225217233893</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>0</v>
       </c>
@@ -602,15 +617,15 @@
       <c r="C6">
         <v>5.0707039999999997E-3</v>
       </c>
-      <c r="E6">
+      <c r="F6">
         <f>(10^C6-1)*100</f>
         <v>1.1744154800775952</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>0</v>
       </c>
@@ -623,15 +638,15 @@
       <c r="D7">
         <v>0.54293340099999998</v>
       </c>
-      <c r="E7">
-        <f t="shared" ref="E7" si="1">(C7/D7)*100</f>
+      <c r="F7">
+        <f t="shared" ref="F7" si="1">(C7/D7)*100</f>
         <v>-0.20413111404800088</v>
       </c>
-      <c r="F7" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>0</v>
       </c>
@@ -641,15 +656,17 @@
       <c r="C8">
         <v>-6.6779830000000002E-3</v>
       </c>
-      <c r="E8">
-        <f>(EXP(C8)-1)*100</f>
-        <v>-0.66557348233888813</v>
-      </c>
-      <c r="F8" t="s">
+      <c r="F8">
+        <v>-0.31914419999999999</v>
+      </c>
+      <c r="G8" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="H8" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>0</v>
       </c>
@@ -659,15 +676,15 @@
       <c r="C9">
         <v>1.0303468E-2</v>
       </c>
-      <c r="E9">
+      <c r="F9">
         <f>(10^C9-1)*100</f>
         <v>2.4008279284029932</v>
       </c>
-      <c r="F9" t="s">
+      <c r="G9" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>0</v>
       </c>
@@ -680,15 +697,15 @@
       <c r="D10">
         <v>0.51791088799999996</v>
       </c>
-      <c r="E10">
-        <f t="shared" ref="E10" si="2">(C10/D10)*100</f>
+      <c r="F10">
+        <f t="shared" ref="F10" si="2">(C10/D10)*100</f>
         <v>-0.2190917446014381</v>
       </c>
-      <c r="F10" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G10" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>0</v>
       </c>
@@ -698,18 +715,18 @@
       <c r="C11">
         <v>6.2631399999999999E-4</v>
       </c>
-      <c r="D11">
-        <v>0.82625772399999997</v>
-      </c>
       <c r="E11">
-        <f>(C11/(D11^2))*100</f>
-        <v>9.1740489876634884E-2</v>
-      </c>
-      <c r="F11" t="s">
+        <v>0.69601350890374436</v>
+      </c>
+      <c r="F11">
+        <f>((C11/2)/E11)*100</f>
+        <v>4.4992948555443661E-2</v>
+      </c>
+      <c r="G11" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>0</v>
       </c>
@@ -720,17 +737,17 @@
         <v>7.8684249999999997E-2</v>
       </c>
       <c r="D12">
-        <v>37.709882800000003</v>
-      </c>
-      <c r="E12">
-        <f t="shared" ref="E12:E14" si="3">(C12/D12)*100</f>
-        <v>0.20865684048214542</v>
-      </c>
-      <c r="F12" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+        <v>39.709882800000003</v>
+      </c>
+      <c r="F12">
+        <f t="shared" ref="F12:F14" si="3">(C12/D12)*100</f>
+        <v>0.19814777695591687</v>
+      </c>
+      <c r="G12" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>0</v>
       </c>
@@ -743,15 +760,16 @@
       <c r="D13" s="1">
         <v>0.29114584599999999</v>
       </c>
-      <c r="E13">
+      <c r="E13" s="1"/>
+      <c r="F13">
         <f t="shared" si="3"/>
         <v>2.7855454959848546E-2</v>
       </c>
-      <c r="F13" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G13" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>0</v>
       </c>
@@ -764,15 +782,15 @@
       <c r="D14">
         <v>1.42520523</v>
       </c>
-      <c r="E14">
+      <c r="F14">
         <f t="shared" si="3"/>
         <v>3.9663594975721499</v>
       </c>
-      <c r="F14" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G14" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>0</v>
       </c>
@@ -782,15 +800,15 @@
       <c r="C15">
         <v>1.6619630999999999E-2</v>
       </c>
-      <c r="E15">
+      <c r="F15">
         <f>(10^C15-1)*100</f>
         <v>3.9009769217007051</v>
       </c>
-      <c r="F15" t="s">
+      <c r="G15" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>0</v>
       </c>
@@ -803,15 +821,15 @@
       <c r="D16">
         <v>27.528243620000001</v>
       </c>
-      <c r="E16">
+      <c r="F16">
         <f>(C16/D16)*100</f>
         <v>0.63768780683291559</v>
       </c>
-      <c r="F16" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G16" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>0</v>
       </c>
@@ -821,15 +839,15 @@
       <c r="C17">
         <v>1.1438570000000001E-3</v>
       </c>
-      <c r="E17">
+      <c r="F17">
         <f>(10^C17-1)*100</f>
         <v>0.26372996490582334</v>
       </c>
-      <c r="F17" t="s">
+      <c r="G17" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>0</v>
       </c>
@@ -842,15 +860,15 @@
       <c r="D18">
         <v>9.2795485230000008</v>
       </c>
-      <c r="E18">
+      <c r="F18">
         <f>(C18/D18)*100</f>
         <v>0.45473544208978312</v>
       </c>
-      <c r="F18" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G18" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>0</v>
       </c>
@@ -860,15 +878,15 @@
       <c r="C19">
         <v>1.0200776E-2</v>
       </c>
-      <c r="E19">
+      <c r="F19">
         <f>(10^C19-1)*100</f>
         <v>2.3766173913215338</v>
       </c>
-      <c r="F19" t="s">
+      <c r="G19" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>0</v>
       </c>
@@ -881,15 +899,15 @@
       <c r="D20">
         <v>19.19656517</v>
       </c>
-      <c r="E20">
+      <c r="F20">
         <f>(C20/D20)*100</f>
         <v>0.70709655502396318</v>
       </c>
-      <c r="F20" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G20" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>0</v>
       </c>
@@ -899,11 +917,11 @@
       <c r="C21">
         <v>6.6121289999999996E-3</v>
       </c>
-      <c r="E21">
+      <c r="F21">
         <f>(10^C21-1)*100</f>
         <v>1.5341480262085039</v>
       </c>
-      <c r="F21" t="s">
+      <c r="G21" t="s">
         <v>26</v>
       </c>
     </row>

</xml_diff>